<commit_message>
pog working threshold stuff
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aviv0\Desktop\Misc\Azrieli\Year4\FinalProject\TasksSim\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD364814-1B83-40C8-963E-2CC7AF5A3277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="2208" yWindow="2544" windowWidth="25128" windowHeight="12120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MaxRuntimeFirst" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +332,150 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>5442282.407409668</v>
+      </c>
+      <c r="B1">
+        <v>0.2</v>
+      </c>
+      <c r="C1">
+        <v>0.3</v>
+      </c>
+      <c r="D1">
+        <v>0.4</v>
+      </c>
+      <c r="E1">
+        <v>0.5</v>
+      </c>
+      <c r="F1">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="G1">
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="H1">
+        <v>0.8</v>
+      </c>
+      <c r="I1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>94973.148147583008</v>
+      </c>
+      <c r="B2">
+        <v>101754362.7781982</v>
+      </c>
+      <c r="C2">
+        <v>103439977.22257081</v>
+      </c>
+      <c r="D2">
+        <v>104039521.85169069</v>
+      </c>
+      <c r="E2">
+        <v>104702866.6664001</v>
+      </c>
+      <c r="F2">
+        <v>102086890.184967</v>
+      </c>
+      <c r="G2">
+        <v>103904323.1474915</v>
+      </c>
+      <c r="H2">
+        <v>104725303.33363651</v>
+      </c>
+      <c r="I2">
+        <v>102799408.7034851</v>
+      </c>
+      <c r="J2">
+        <v>103921255.37055659</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>11745880.555557249</v>
+      </c>
+      <c r="B3">
+        <v>104101626.1104065</v>
+      </c>
+      <c r="C3">
+        <v>102955019.444519</v>
+      </c>
+      <c r="D3">
+        <v>103506021.8514282</v>
+      </c>
+      <c r="E3">
+        <v>105319586.8520508</v>
+      </c>
+      <c r="F3">
+        <v>103442001.8518005</v>
+      </c>
+      <c r="G3">
+        <v>105554180.9261536</v>
+      </c>
+      <c r="H3">
+        <v>103402012.2221252</v>
+      </c>
+      <c r="I3">
+        <v>103384954.073938</v>
+      </c>
+      <c r="J3">
+        <v>104236394.4444702</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>101889940.9261353</v>
+      </c>
+      <c r="C4">
+        <v>104131162.7781616</v>
+      </c>
+      <c r="D4">
+        <v>103218751.851355</v>
+      </c>
+      <c r="E4">
+        <v>103204377.77811889</v>
+      </c>
+      <c r="F4">
+        <v>101136545.55504151</v>
+      </c>
+      <c r="G4">
+        <v>104416279.4444824</v>
+      </c>
+      <c r="H4">
+        <v>103793333.70430911</v>
+      </c>
+      <c r="I4">
+        <v>103735048.8889709</v>
+      </c>
+      <c r="J4">
+        <v>101922700.0005554</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added is_moblieye to heuristics and fixed run_sim_once but something ain't right
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -3226,6 +3226,15 @@
           <t>gsf.000390.prof.json</t>
         </is>
       </c>
+      <c r="B393" t="n">
+        <v>1</v>
+      </c>
+      <c r="C393" t="n">
+        <v>1</v>
+      </c>
+      <c r="D393" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">

</xml_diff>

<commit_message>
fixed decide of heuristics
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -496,22 +496,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1" s="9" t="n">
         <v>1</v>
       </c>
       <c r="E1" s="9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F1" s="9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G1" s="9" t="n">
         <v>1</v>
       </c>
       <c r="H1" s="9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1">
@@ -8120,25 +8120,25 @@
     <row r="1" ht="18.75" customHeight="1">
       <c r="A1" s="9" t="n"/>
       <c r="B1" s="9" t="n">
-        <v>331.4814453125</v>
+        <v>4832.407409667969</v>
       </c>
       <c r="C1" s="9" t="n">
-        <v>24029.6296081543</v>
+        <v>43790.74072265625</v>
       </c>
       <c r="D1" s="9" t="n">
-        <v>691823.1480712891</v>
+        <v>231532.4074707031</v>
       </c>
       <c r="E1" s="9" t="n">
-        <v>182823.1481628418</v>
+        <v>322.2222900390625</v>
       </c>
       <c r="F1" s="9" t="n">
-        <v>1157.407348632812</v>
+        <v>808.3333435058594</v>
       </c>
       <c r="G1" s="9" t="n">
-        <v>48454.62963867188</v>
+        <v>20832.40740966797</v>
       </c>
       <c r="H1" s="9" t="n">
-        <v>2207.407470703125</v>
+        <v>24772.22229003906</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1">
@@ -8315,27 +8315,13 @@
           <t>gsf.000005.prof.json</t>
         </is>
       </c>
-      <c r="B8" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="B8" s="9" t="n"/>
+      <c r="C8" s="9" t="n"/>
+      <c r="D8" s="9" t="n"/>
+      <c r="E8" s="9" t="n"/>
+      <c r="F8" s="9" t="n"/>
+      <c r="G8" s="9" t="n"/>
+      <c r="H8" s="9" t="n"/>
     </row>
     <row r="9" ht="18.75" customHeight="1">
       <c r="A9" s="9" t="inlineStr">
@@ -8343,27 +8329,13 @@
           <t>gsf.000006.prof.json</t>
         </is>
       </c>
-      <c r="B9" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="B9" s="9" t="n"/>
+      <c r="C9" s="9" t="n"/>
+      <c r="D9" s="9" t="n"/>
+      <c r="E9" s="9" t="n"/>
+      <c r="F9" s="9" t="n"/>
+      <c r="G9" s="9" t="n"/>
+      <c r="H9" s="9" t="n"/>
     </row>
     <row r="10" ht="18.75" customHeight="1">
       <c r="A10" s="9" t="inlineStr">
@@ -8371,27 +8343,13 @@
           <t>gsf.000007.prof.json</t>
         </is>
       </c>
-      <c r="B10" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="B10" s="9" t="n"/>
+      <c r="C10" s="9" t="n"/>
+      <c r="D10" s="9" t="n"/>
+      <c r="E10" s="9" t="n"/>
+      <c r="F10" s="9" t="n"/>
+      <c r="G10" s="9" t="n"/>
+      <c r="H10" s="9" t="n"/>
     </row>
     <row r="11" ht="18.75" customHeight="1">
       <c r="A11" s="9" t="inlineStr">
@@ -8399,27 +8357,13 @@
           <t>gsf.000008.prof.json</t>
         </is>
       </c>
-      <c r="B11" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F11" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="B11" s="9" t="n"/>
+      <c r="C11" s="9" t="n"/>
+      <c r="D11" s="9" t="n"/>
+      <c r="E11" s="9" t="n"/>
+      <c r="F11" s="9" t="n"/>
+      <c r="G11" s="9" t="n"/>
+      <c r="H11" s="9" t="n"/>
     </row>
     <row r="12" ht="18.75" customHeight="1">
       <c r="A12" s="9" t="inlineStr">
@@ -8427,27 +8371,13 @@
           <t>gsf.000009.prof.json</t>
         </is>
       </c>
-      <c r="B12" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="B12" s="9" t="n"/>
+      <c r="C12" s="9" t="n"/>
+      <c r="D12" s="9" t="n"/>
+      <c r="E12" s="9" t="n"/>
+      <c r="F12" s="9" t="n"/>
+      <c r="G12" s="9" t="n"/>
+      <c r="H12" s="9" t="n"/>
     </row>
     <row r="13" ht="18.75" customHeight="1">
       <c r="A13" s="9" t="inlineStr">
@@ -8455,27 +8385,13 @@
           <t>gsf.000010.prof.json</t>
         </is>
       </c>
-      <c r="B13" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="B13" s="9" t="n"/>
+      <c r="C13" s="9" t="n"/>
+      <c r="D13" s="9" t="n"/>
+      <c r="E13" s="9" t="n"/>
+      <c r="F13" s="9" t="n"/>
+      <c r="G13" s="9" t="n"/>
+      <c r="H13" s="9" t="n"/>
     </row>
     <row r="14" ht="18.75" customHeight="1">
       <c r="A14" s="9" t="inlineStr">
@@ -8483,27 +8399,13 @@
           <t>gsf.000011.prof.json</t>
         </is>
       </c>
-      <c r="B14" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E14" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F14" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G14" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="B14" s="9" t="n"/>
+      <c r="C14" s="9" t="n"/>
+      <c r="D14" s="9" t="n"/>
+      <c r="E14" s="9" t="n"/>
+      <c r="F14" s="9" t="n"/>
+      <c r="G14" s="9" t="n"/>
+      <c r="H14" s="9" t="n"/>
     </row>
     <row r="15" ht="18.75" customHeight="1">
       <c r="A15" s="9" t="inlineStr">
@@ -8511,27 +8413,13 @@
           <t>gsf.000012.prof.json</t>
         </is>
       </c>
-      <c r="B15" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G15" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H15" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="B15" s="9" t="n"/>
+      <c r="C15" s="9" t="n"/>
+      <c r="D15" s="9" t="n"/>
+      <c r="E15" s="9" t="n"/>
+      <c r="F15" s="9" t="n"/>
+      <c r="G15" s="9" t="n"/>
+      <c r="H15" s="9" t="n"/>
     </row>
     <row r="16" ht="18.75" customHeight="1">
       <c r="A16" s="9" t="inlineStr">
@@ -8539,27 +8427,13 @@
           <t>gsf.000013.prof.json</t>
         </is>
       </c>
-      <c r="B16" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G16" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H16" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="B16" s="9" t="n"/>
+      <c r="C16" s="9" t="n"/>
+      <c r="D16" s="9" t="n"/>
+      <c r="E16" s="9" t="n"/>
+      <c r="F16" s="9" t="n"/>
+      <c r="G16" s="9" t="n"/>
+      <c r="H16" s="9" t="n"/>
     </row>
     <row r="17" ht="18.75" customHeight="1">
       <c r="A17" s="9" t="inlineStr">
@@ -8567,27 +8441,13 @@
           <t>gsf.000014.prof.json</t>
         </is>
       </c>
-      <c r="B17" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D17" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G17" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H17" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="B17" s="9" t="n"/>
+      <c r="C17" s="9" t="n"/>
+      <c r="D17" s="9" t="n"/>
+      <c r="E17" s="9" t="n"/>
+      <c r="F17" s="9" t="n"/>
+      <c r="G17" s="9" t="n"/>
+      <c r="H17" s="9" t="n"/>
     </row>
     <row r="18" ht="18.75" customHeight="1">
       <c r="A18" s="9" t="inlineStr">
@@ -8595,27 +8455,13 @@
           <t>gsf.000015.prof.json</t>
         </is>
       </c>
-      <c r="B18" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E18" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G18" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H18" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="B18" s="9" t="n"/>
+      <c r="C18" s="9" t="n"/>
+      <c r="D18" s="9" t="n"/>
+      <c r="E18" s="9" t="n"/>
+      <c r="F18" s="9" t="n"/>
+      <c r="G18" s="9" t="n"/>
+      <c r="H18" s="9" t="n"/>
     </row>
     <row r="19" ht="18.75" customHeight="1">
       <c r="A19" s="9" t="inlineStr">
@@ -8623,27 +8469,13 @@
           <t>gsf.000016.prof.json</t>
         </is>
       </c>
-      <c r="B19" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E19" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G19" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H19" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="B19" s="9" t="n"/>
+      <c r="C19" s="9" t="n"/>
+      <c r="D19" s="9" t="n"/>
+      <c r="E19" s="9" t="n"/>
+      <c r="F19" s="9" t="n"/>
+      <c r="G19" s="9" t="n"/>
+      <c r="H19" s="9" t="n"/>
     </row>
     <row r="20" ht="18.75" customHeight="1">
       <c r="A20" s="9" t="inlineStr">
@@ -8651,27 +8483,13 @@
           <t>gsf.000017.prof.json</t>
         </is>
       </c>
-      <c r="B20" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D20" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E20" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F20" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G20" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H20" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="B20" s="9" t="n"/>
+      <c r="C20" s="9" t="n"/>
+      <c r="D20" s="9" t="n"/>
+      <c r="E20" s="9" t="n"/>
+      <c r="F20" s="9" t="n"/>
+      <c r="G20" s="9" t="n"/>
+      <c r="H20" s="9" t="n"/>
     </row>
     <row r="21" ht="18.75" customHeight="1">
       <c r="A21" s="9" t="inlineStr">
@@ -8679,27 +8497,13 @@
           <t>gsf.000018.prof.json</t>
         </is>
       </c>
-      <c r="B21" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E21" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F21" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G21" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H21" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="B21" s="9" t="n"/>
+      <c r="C21" s="9" t="n"/>
+      <c r="D21" s="9" t="n"/>
+      <c r="E21" s="9" t="n"/>
+      <c r="F21" s="9" t="n"/>
+      <c r="G21" s="9" t="n"/>
+      <c r="H21" s="9" t="n"/>
     </row>
     <row r="22" ht="18.75" customHeight="1">
       <c r="A22" s="9" t="inlineStr">
@@ -8707,27 +8511,13 @@
           <t>gsf.000019.prof.json</t>
         </is>
       </c>
-      <c r="B22" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E22" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F22" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G22" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H22" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="B22" s="9" t="n"/>
+      <c r="C22" s="9" t="n"/>
+      <c r="D22" s="9" t="n"/>
+      <c r="E22" s="9" t="n"/>
+      <c r="F22" s="9" t="n"/>
+      <c r="G22" s="9" t="n"/>
+      <c r="H22" s="9" t="n"/>
     </row>
     <row r="23" ht="18.75" customHeight="1">
       <c r="A23" s="9" t="inlineStr">
@@ -8735,18 +8525,10 @@
           <t>gsf.000020.prof.json</t>
         </is>
       </c>
-      <c r="B23" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="B23" s="9" t="n"/>
+      <c r="C23" s="9" t="n"/>
+      <c r="D23" s="9" t="n"/>
+      <c r="E23" s="9" t="n"/>
       <c r="F23" s="9" t="n"/>
       <c r="G23" s="9" t="n"/>
       <c r="H23" s="9" t="n"/>
@@ -16049,25 +15831,25 @@
     <row r="1" ht="18.75" customHeight="1">
       <c r="A1" s="9" t="n"/>
       <c r="B1" s="9" t="n">
-        <v>331.4814453125</v>
+        <v>4832.407409667969</v>
       </c>
       <c r="C1" s="9" t="n">
-        <v>24029.6296081543</v>
+        <v>43790.74072265625</v>
       </c>
       <c r="D1" s="9" t="n">
-        <v>691823.1480712891</v>
+        <v>231532.4074707031</v>
       </c>
       <c r="E1" s="9" t="n">
-        <v>182823.1481628418</v>
+        <v>322.2222900390625</v>
       </c>
       <c r="F1" s="9" t="n">
-        <v>1157.407348632812</v>
+        <v>808.3333435058594</v>
       </c>
       <c r="G1" s="9" t="n">
-        <v>48454.62963867188</v>
+        <v>20832.40740966797</v>
       </c>
       <c r="H1" s="9" t="n">
-        <v>2207.407470703125</v>
+        <v>24772.22229003906</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1">
@@ -23679,22 +23461,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1" s="9" t="n">
         <v>1</v>
       </c>
       <c r="E1" s="9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F1" s="9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G1" s="9" t="n">
         <v>1</v>
       </c>
       <c r="H1" s="9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1">

</xml_diff>